<commit_message>
Initi figs, 30tr results
</commit_message>
<xml_diff>
--- a/results/20n6r_fails025_tasks0_2Stg.xlsx
+++ b/results/20n6r_fails025_tasks0_2Stg.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RDML\Documents\MOTHERSHIP\masop\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2989BB57-5B99-4C0E-B86E-EB543D6ABC16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-15360" yWindow="132" windowWidth="15360" windowHeight="8340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,94 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+  <si>
+    <t>twoStep_rew</t>
+  </si>
+  <si>
+    <t>twoStep_potent</t>
+  </si>
+  <si>
+    <t>twoStep_percDead</t>
+  </si>
+  <si>
+    <t>0.8111111111111111</t>
+  </si>
+  <si>
+    <t>0.3333333333333333</t>
+  </si>
+  <si>
+    <t>0.6304347826086957</t>
+  </si>
+  <si>
+    <t>0.7282608695652174</t>
+  </si>
+  <si>
+    <t>0.42105263157894735</t>
+  </si>
+  <si>
+    <t>0.6491228070175439</t>
+  </si>
+  <si>
+    <t>0.5925925925925926</t>
+  </si>
+  <si>
+    <t>0.8024691358024691</t>
+  </si>
+  <si>
+    <t>0.7008547008547008</t>
+  </si>
+  <si>
+    <t>0.7777777777777778</t>
+  </si>
+  <si>
+    <t>0.8709677419354839</t>
+  </si>
+  <si>
+    <t>0.7543859649122807</t>
+  </si>
+  <si>
+    <t>0.9035087719298246</t>
+  </si>
+  <si>
+    <t>0.45555555555555555</t>
+  </si>
+  <si>
+    <t>0.8222222222222222</t>
+  </si>
+  <si>
+    <t>0.21153846153846154</t>
+  </si>
+  <si>
+    <t>0.6666666666666666</t>
+  </si>
+  <si>
+    <t>0.8387096774193549</t>
+  </si>
+  <si>
+    <t>0.8245614035087719</t>
+  </si>
+  <si>
+    <t>0.9473684210526315</t>
+  </si>
+  <si>
+    <t>0.6470588235294118</t>
+  </si>
+  <si>
+    <t>0.8021978021978022</t>
+  </si>
+  <si>
+    <t>0.9230769230769231</t>
+  </si>
+  <si>
+    <t>0.35514018691588783</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +141,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +423,181 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>0.71962616822429903</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>